<commit_message>
added execution time analysis for block processing
</commit_message>
<xml_diff>
--- a/speed-up stats.xlsx
+++ b/speed-up stats.xlsx
@@ -3,7 +3,7 @@
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
   <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="19126"/>
   <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{4C62B3BE-9B63-4758-9D00-22D33B48DF73}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="10_ncr:100000_{B50A7A3E-AEBB-4864-8BA2-1813D0197602}" xr6:coauthVersionLast="31" xr6:coauthVersionMax="31" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12645" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,7 +20,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="14">
   <si>
     <t>OpenMPI</t>
   </si>
@@ -56,6 +56,12 @@
   </si>
   <si>
     <t>var nodes</t>
+  </si>
+  <si>
+    <t>block dec</t>
+  </si>
+  <si>
+    <t>block enc</t>
   </si>
 </sst>
 </file>
@@ -376,8 +382,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H68"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E14" sqref="E14"/>
+    <sheetView tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="G34" sqref="G34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -418,7 +424,7 @@
         <v>2.0419000000000001E-3</v>
       </c>
       <c r="F4">
-        <v>0.19365299999999999</v>
+        <v>0.71687699999999999</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.25">
@@ -435,7 +441,7 @@
         <v>1.0975099999999999E-3</v>
       </c>
       <c r="F5">
-        <v>0.22674900000000001</v>
+        <v>1.682831</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.25">
@@ -452,7 +458,7 @@
         <v>7.3984599999999995E-4</v>
       </c>
       <c r="F6">
-        <v>0.164823</v>
+        <v>1.344659</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.25">
@@ -469,7 +475,7 @@
         <v>5.9224799999999997E-4</v>
       </c>
       <c r="F7">
-        <v>0.121223</v>
+        <v>1.0164169999999999</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.25">
@@ -486,7 +492,7 @@
         <v>6.6664999999999997E-4</v>
       </c>
       <c r="F8">
-        <v>0.104314</v>
+        <v>0.92001200000000005</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.25">
@@ -503,7 +509,7 @@
         <v>7.7366399999999997E-4</v>
       </c>
       <c r="F9">
-        <v>0.100951</v>
+        <v>0.75994300000000004</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.25">
@@ -520,7 +526,7 @@
         <v>2.7223500000000001E-3</v>
       </c>
       <c r="F11">
-        <v>0.12703500000000001</v>
+        <v>0.452484</v>
       </c>
     </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.25">
@@ -537,7 +543,7 @@
         <v>1.54382E-3</v>
       </c>
       <c r="F12">
-        <v>0.15492700000000001</v>
+        <v>0.88073100000000004</v>
       </c>
     </row>
     <row r="13" spans="1:6" x14ac:dyDescent="0.25">
@@ -554,7 +560,7 @@
         <v>8.3998299999999998E-4</v>
       </c>
       <c r="F13">
-        <v>0.114</v>
+        <v>0.90010800000000002</v>
       </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.25">
@@ -571,7 +577,7 @@
         <v>8.0500000000000005E-4</v>
       </c>
       <c r="F14">
-        <v>8.5485400000000003E-2</v>
+        <v>0.71859499999999998</v>
       </c>
     </row>
     <row r="15" spans="1:6" x14ac:dyDescent="0.25">
@@ -588,7 +594,7 @@
         <v>7.2425899999999999E-4</v>
       </c>
       <c r="F15">
-        <v>6.9310099999999999E-2</v>
+        <v>0.59260400000000002</v>
       </c>
     </row>
     <row r="16" spans="1:6" x14ac:dyDescent="0.25">
@@ -605,10 +611,10 @@
         <v>1.0118799999999999E-3</v>
       </c>
       <c r="F16">
-        <v>7.8571199999999994E-2</v>
-      </c>
-    </row>
-    <row r="18" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.52169600000000005</v>
+      </c>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18">
         <v>1</v>
       </c>
@@ -622,10 +628,10 @@
         <v>2.29502E-3</v>
       </c>
       <c r="F18">
-        <v>6.45342E-2</v>
-      </c>
-    </row>
-    <row r="19" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.218838</v>
+      </c>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19">
         <v>2</v>
       </c>
@@ -639,10 +645,10 @@
         <v>1.3208199999999999E-3</v>
       </c>
       <c r="F19">
-        <v>6.60303E-2</v>
-      </c>
-    </row>
-    <row r="20" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.59319699999999997</v>
+      </c>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20">
         <v>4</v>
       </c>
@@ -656,10 +662,10 @@
         <v>6.7701000000000002E-4</v>
       </c>
       <c r="F20">
-        <v>6.0712799999999997E-2</v>
-      </c>
-    </row>
-    <row r="21" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.48139100000000001</v>
+      </c>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21">
         <v>8</v>
       </c>
@@ -673,10 +679,10 @@
         <v>5.9862399999999997E-4</v>
       </c>
       <c r="F21">
-        <v>4.8501799999999998E-2</v>
-      </c>
-    </row>
-    <row r="22" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.36499199999999998</v>
+      </c>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22">
         <v>16</v>
       </c>
@@ -690,10 +696,10 @@
         <v>1.2283999999999999E-3</v>
       </c>
       <c r="F22">
-        <v>4.30561E-2</v>
-      </c>
-    </row>
-    <row r="23" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.30582300000000001</v>
+      </c>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23">
         <v>32</v>
       </c>
@@ -707,18 +713,24 @@
         <v>1.56201E-3</v>
       </c>
       <c r="F23">
-        <v>4.9449100000000003E-2</v>
-      </c>
-    </row>
-    <row r="26" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.27196300000000001</v>
+      </c>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>1</v>
       </c>
       <c r="B26" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="27" spans="1:6" x14ac:dyDescent="0.25">
+      <c r="G26" t="s">
+        <v>13</v>
+      </c>
+      <c r="H26" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27">
         <v>1</v>
       </c>
@@ -732,10 +744,16 @@
         <v>4.9827000000000003E-5</v>
       </c>
       <c r="F27">
-        <v>2.4168499999999999E-2</v>
-      </c>
-    </row>
-    <row r="28" spans="1:6" x14ac:dyDescent="0.25">
+        <v>8.2965999999999998E-2</v>
+      </c>
+      <c r="G27">
+        <v>1.0779E-2</v>
+      </c>
+      <c r="H27">
+        <v>27.773484</v>
+      </c>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28">
         <v>2</v>
       </c>
@@ -749,10 +767,16 @@
         <v>5.8081000000000002E-5</v>
       </c>
       <c r="F28">
-        <v>2.5496600000000001E-2</v>
-      </c>
-    </row>
-    <row r="29" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.17172399999999999</v>
+      </c>
+      <c r="G28">
+        <v>6.2370000000000004E-3</v>
+      </c>
+      <c r="H28">
+        <v>13.993944000000001</v>
+      </c>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29">
         <v>4</v>
       </c>
@@ -766,10 +790,16 @@
         <v>5.3186000000000002E-5</v>
       </c>
       <c r="F29">
-        <v>2.0400999999999999E-2</v>
-      </c>
-    </row>
-    <row r="30" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.154365</v>
+      </c>
+      <c r="G29">
+        <v>3.5829999999999998E-3</v>
+      </c>
+      <c r="H29">
+        <v>7.3988149999999999</v>
+      </c>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30">
         <v>8</v>
       </c>
@@ -783,10 +813,16 @@
         <v>9.1000000000000003E-5</v>
       </c>
       <c r="F30">
-        <v>1.6212799999999999E-2</v>
-      </c>
-    </row>
-    <row r="31" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.113423</v>
+      </c>
+      <c r="G30">
+        <v>2.3730000000000001E-3</v>
+      </c>
+      <c r="H30">
+        <v>4.0905139999999998</v>
+      </c>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31">
         <v>16</v>
       </c>
@@ -800,10 +836,16 @@
         <v>6.0784399999999996E-4</v>
       </c>
       <c r="F31">
-        <v>1.6349499999999999E-2</v>
-      </c>
-    </row>
-    <row r="32" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.11387</v>
+      </c>
+      <c r="G31">
+        <v>2.8379999999999998E-3</v>
+      </c>
+      <c r="H31">
+        <v>2.4625020000000002</v>
+      </c>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32">
         <v>32</v>
       </c>
@@ -817,10 +859,16 @@
         <v>7.9199999999999995E-4</v>
       </c>
       <c r="F32">
-        <v>1.2539399999999999E-2</v>
-      </c>
-    </row>
-    <row r="34" spans="1:6" x14ac:dyDescent="0.25">
+        <v>9.4001000000000001E-2</v>
+      </c>
+      <c r="G32">
+        <v>2.349E-3</v>
+      </c>
+      <c r="H32">
+        <v>1.604671</v>
+      </c>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34">
         <v>1</v>
       </c>
@@ -834,10 +882,16 @@
         <v>5.04496E-4</v>
       </c>
       <c r="F34">
-        <v>9.6235899999999999E-2</v>
-      </c>
-    </row>
-    <row r="35" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.34893299999999999</v>
+      </c>
+      <c r="G34">
+        <v>0.163467</v>
+      </c>
+      <c r="H34">
+        <v>115.57890399999999</v>
+      </c>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35">
         <v>2</v>
       </c>
@@ -851,10 +905,16 @@
         <v>2.9539600000000002E-4</v>
       </c>
       <c r="F35">
-        <v>0.113175</v>
-      </c>
-    </row>
-    <row r="36" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.67353200000000002</v>
+      </c>
+      <c r="G35">
+        <v>8.2957000000000003E-2</v>
+      </c>
+      <c r="H35">
+        <v>57.757938000000003</v>
+      </c>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36">
         <v>4</v>
       </c>
@@ -868,10 +928,16 @@
         <v>1.8453100000000001E-4</v>
       </c>
       <c r="F36">
-        <v>8.2817500000000002E-2</v>
-      </c>
-    </row>
-    <row r="37" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.651806</v>
+      </c>
+      <c r="G36">
+        <v>4.3014999999999998E-2</v>
+      </c>
+      <c r="H36">
+        <v>30.707094999999999</v>
+      </c>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37">
         <v>8</v>
       </c>
@@ -885,10 +951,16 @@
         <v>1.8769500000000001E-4</v>
       </c>
       <c r="F37">
-        <v>6.3916100000000003E-2</v>
-      </c>
-    </row>
-    <row r="38" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.52751499999999996</v>
+      </c>
+      <c r="G37">
+        <v>2.5579999999999999E-2</v>
+      </c>
+      <c r="H37">
+        <v>16.400642000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38">
         <v>16</v>
       </c>
@@ -902,10 +974,16 @@
         <v>6.8185700000000001E-4</v>
       </c>
       <c r="F38">
-        <v>5.1121300000000001E-2</v>
-      </c>
-    </row>
-    <row r="39" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.41630699999999998</v>
+      </c>
+      <c r="G38">
+        <v>1.7742999999999998E-2</v>
+      </c>
+      <c r="H38">
+        <v>9.0633820000000007</v>
+      </c>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39">
         <v>32</v>
       </c>
@@ -919,10 +997,16 @@
         <v>9.2643800000000002E-4</v>
       </c>
       <c r="F39">
-        <v>5.6354899999999999E-2</v>
-      </c>
-    </row>
-    <row r="41" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.389791</v>
+      </c>
+      <c r="G39">
+        <v>1.7295000000000001E-2</v>
+      </c>
+      <c r="H39">
+        <v>6.6783279999999996</v>
+      </c>
+    </row>
+    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A41">
         <v>1</v>
       </c>
@@ -936,10 +1020,16 @@
         <v>2.0419000000000001E-3</v>
       </c>
       <c r="F41">
-        <v>0.19365299999999999</v>
-      </c>
-    </row>
-    <row r="42" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.71687699999999999</v>
+      </c>
+      <c r="G41">
+        <v>0.65625199999999995</v>
+      </c>
+      <c r="H41">
+        <v>233.13479000000001</v>
+      </c>
+    </row>
+    <row r="42" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A42">
         <v>2</v>
       </c>
@@ -953,10 +1043,16 @@
         <v>1.0975099999999999E-3</v>
       </c>
       <c r="F42">
-        <v>0.22674900000000001</v>
-      </c>
-    </row>
-    <row r="43" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.682831</v>
+      </c>
+      <c r="G42">
+        <v>0.32892500000000002</v>
+      </c>
+      <c r="H42">
+        <v>119.174823</v>
+      </c>
+    </row>
+    <row r="43" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A43">
         <v>4</v>
       </c>
@@ -970,10 +1066,16 @@
         <v>7.3984599999999995E-4</v>
       </c>
       <c r="F43">
-        <v>0.164823</v>
-      </c>
-    </row>
-    <row r="44" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.344659</v>
+      </c>
+      <c r="G43">
+        <v>0.18026</v>
+      </c>
+      <c r="H43">
+        <v>64.143503999999993</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A44">
         <v>8</v>
       </c>
@@ -987,10 +1089,16 @@
         <v>5.9224799999999997E-4</v>
       </c>
       <c r="F44">
-        <v>0.121223</v>
-      </c>
-    </row>
-    <row r="45" spans="1:6" x14ac:dyDescent="0.25">
+        <v>1.0164169999999999</v>
+      </c>
+      <c r="G44">
+        <v>9.6229999999999996E-2</v>
+      </c>
+      <c r="H44">
+        <v>33.268712000000001</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A45">
         <v>16</v>
       </c>
@@ -1004,10 +1112,16 @@
         <v>6.6664999999999997E-4</v>
       </c>
       <c r="F45">
-        <v>0.104314</v>
-      </c>
-    </row>
-    <row r="46" spans="1:6" x14ac:dyDescent="0.25">
+        <v>0.92001200000000005</v>
+      </c>
+      <c r="G45">
+        <v>8.5880999999999999E-2</v>
+      </c>
+      <c r="H45">
+        <v>25.402884</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A46">
         <v>32</v>
       </c>
@@ -1021,7 +1135,13 @@
         <v>7.7366399999999997E-4</v>
       </c>
       <c r="F46">
-        <v>0.100951</v>
+        <v>0.75994300000000004</v>
+      </c>
+      <c r="G46">
+        <v>5.3106E-2</v>
+      </c>
+      <c r="H46">
+        <v>16.854669000000001</v>
       </c>
     </row>
     <row r="50" spans="1:8" x14ac:dyDescent="0.25">

</xml_diff>